<commit_message>
Thank You for Choosing to Learn from in28Minutes
</commit_message>
<xml_diff>
--- a/web-driver-4-data-driven-tests/src/test/resources/login-data.xlsx
+++ b/web-driver-4-data-driven-tests/src/test/resources/login-data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>in28minutes</t>
   </si>
@@ -19,19 +19,13 @@
     <t>dummy</t>
   </si>
   <si>
-    <t>wrongpassword</t>
-  </si>
-  <si>
     <t>adam</t>
   </si>
   <si>
-    <t>adamworng</t>
+    <t>adam@123</t>
   </si>
   <si>
     <t>eve</t>
-  </si>
-  <si>
-    <t>eve@123</t>
   </si>
 </sst>
 </file>
@@ -102,7 +96,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -113,68 +107,24 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C3" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="1" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>